<commit_message>
removed line 122, added all stdev's and categorizations except for those from experiment 38 and for those whose experiment #'s not present; will be resolved when lab notebook acquired.
</commit_message>
<xml_diff>
--- a/expdata_metafile_FEB_08_2022.xlsx
+++ b/expdata_metafile_FEB_08_2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naazb\thermal-experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E034297C-5092-4312-A2F5-5FF1C95F760C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6834A057-2DD9-4C99-BE8A-7594664BD8B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1036C2BD-7801-48B2-9F85-BAB75D33EE99}"/>
+    <workbookView xWindow="36" yWindow="108" windowWidth="11460" windowHeight="6000" xr2:uid="{1036C2BD-7801-48B2-9F85-BAB75D33EE99}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="123">
   <si>
     <t>Experiment_Number</t>
   </si>
@@ -391,12 +391,6 @@
   </si>
   <si>
     <t>Simplelong27_000_15</t>
-  </si>
-  <si>
-    <t>Simplelong27_095_1</t>
-  </si>
-  <si>
-    <t>contamination</t>
   </si>
   <si>
     <t>Simplelong27_000_16</t>
@@ -762,28 +756,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80E89A6-1830-4F9F-B29F-04DB581FD91D}">
-  <dimension ref="A1:P124"/>
+  <dimension ref="A1:P123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="119" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K129" sqref="K129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
-    <col min="2" max="2" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="18.44140625" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="19.109375" customWidth="1"/>
     <col min="4" max="4" width="21.77734375" customWidth="1"/>
     <col min="5" max="5" width="24.6640625" customWidth="1"/>
     <col min="6" max="6" width="16.88671875" customWidth="1"/>
     <col min="7" max="7" width="18.88671875" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
-    <col min="9" max="9" width="16.109375" customWidth="1"/>
-    <col min="10" max="10" width="14.88671875" customWidth="1"/>
-    <col min="11" max="11" width="12" customWidth="1"/>
-    <col min="12" max="12" width="10.77734375" customWidth="1"/>
-    <col min="13" max="13" width="16.109375" customWidth="1"/>
-    <col min="14" max="14" width="5.5546875" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="16.21875" customWidth="1"/>
+    <col min="13" max="13" width="12.5546875" customWidth="1"/>
+    <col min="14" max="14" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -830,10 +824,10 @@
         <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="P1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -1090,8 +1084,12 @@
       <c r="N8" t="s">
         <v>22</v>
       </c>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="O8" s="2">
+        <v>2.52</v>
+      </c>
+      <c r="P8" s="2">
+        <v>2.5099999999999998</v>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -1127,8 +1125,12 @@
       <c r="N9" t="s">
         <v>24</v>
       </c>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="O9" s="2">
+        <v>2.52</v>
+      </c>
+      <c r="P9" s="2">
+        <v>2.5299999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10">
@@ -4284,8 +4286,12 @@
       <c r="N84" t="s">
         <v>15</v>
       </c>
-      <c r="O84" s="2"/>
-      <c r="P84" s="2"/>
+      <c r="O84" s="2">
+        <v>1.94</v>
+      </c>
+      <c r="P84" s="2">
+        <v>2.14</v>
+      </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A85">
@@ -4321,8 +4327,12 @@
       <c r="N85" t="s">
         <v>22</v>
       </c>
-      <c r="O85" s="2"/>
-      <c r="P85" s="2"/>
+      <c r="O85" s="2">
+        <v>1.77</v>
+      </c>
+      <c r="P85" s="2">
+        <v>1.88</v>
+      </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A86">
@@ -4404,8 +4414,12 @@
       <c r="N87" t="s">
         <v>15</v>
       </c>
-      <c r="O87" s="2"/>
-      <c r="P87" s="2"/>
+      <c r="O87" s="2">
+        <v>2.27</v>
+      </c>
+      <c r="P87" s="2">
+        <v>2.15</v>
+      </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A88">
@@ -4493,8 +4507,12 @@
       <c r="N89" t="s">
         <v>24</v>
       </c>
-      <c r="O89" s="2"/>
-      <c r="P89" s="2"/>
+      <c r="O89" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="P89" s="2">
+        <v>3.02</v>
+      </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A90">
@@ -4672,8 +4690,12 @@
       <c r="N94" t="s">
         <v>22</v>
       </c>
-      <c r="O94" s="2"/>
-      <c r="P94" s="2"/>
+      <c r="O94" s="2">
+        <v>2.57</v>
+      </c>
+      <c r="P94" s="2">
+        <v>3.1</v>
+      </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A95">
@@ -4709,8 +4731,12 @@
       <c r="N95" t="s">
         <v>22</v>
       </c>
-      <c r="O95" s="2"/>
-      <c r="P95" s="2"/>
+      <c r="O95" s="2">
+        <v>3.06</v>
+      </c>
+      <c r="P95" s="2">
+        <v>2.88</v>
+      </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A96">
@@ -4755,8 +4781,12 @@
       <c r="N96" t="s">
         <v>15</v>
       </c>
-      <c r="O96" s="2"/>
-      <c r="P96" s="2"/>
+      <c r="O96" s="2">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="P96" s="2">
+        <v>2.1800000000000002</v>
+      </c>
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A97">
@@ -4847,8 +4877,12 @@
       <c r="N98" t="s">
         <v>24</v>
       </c>
-      <c r="O98" s="2"/>
-      <c r="P98" s="2"/>
+      <c r="O98" s="2">
+        <v>2.48</v>
+      </c>
+      <c r="P98" s="2">
+        <v>2.52</v>
+      </c>
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B99">
@@ -5059,8 +5093,12 @@
       <c r="N103" t="s">
         <v>24</v>
       </c>
-      <c r="O103" s="2"/>
-      <c r="P103" s="2"/>
+      <c r="O103" s="2">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="P103" s="2">
+        <v>2.48</v>
+      </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A104">
@@ -5105,8 +5143,12 @@
       <c r="N104" t="s">
         <v>22</v>
       </c>
-      <c r="O104" s="2"/>
-      <c r="P104" s="2"/>
+      <c r="O104" s="2">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="P104" s="2">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A105">
@@ -5151,8 +5193,12 @@
       <c r="N105" t="s">
         <v>24</v>
       </c>
-      <c r="O105" s="2"/>
-      <c r="P105" s="2"/>
+      <c r="O105" s="2">
+        <v>2.48</v>
+      </c>
+      <c r="P105" s="2">
+        <v>2.4900000000000002</v>
+      </c>
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A106">
@@ -5243,8 +5289,12 @@
       <c r="N107" t="s">
         <v>15</v>
       </c>
-      <c r="O107" s="2"/>
-      <c r="P107" s="2"/>
+      <c r="O107" s="2">
+        <v>2.04</v>
+      </c>
+      <c r="P107" s="2">
+        <v>2.16</v>
+      </c>
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B108">
@@ -5844,16 +5894,31 @@
         <v>119</v>
       </c>
       <c r="F122">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="G122">
-        <v>4</v>
-      </c>
-      <c r="K122" t="s">
-        <v>120</v>
+        <v>5</v>
+      </c>
+      <c r="H122">
+        <v>18</v>
+      </c>
+      <c r="I122">
+        <v>18</v>
+      </c>
+      <c r="J122">
+        <v>9</v>
+      </c>
+      <c r="K122">
+        <v>8</v>
+      </c>
+      <c r="L122">
+        <v>8</v>
+      </c>
+      <c r="M122">
+        <v>8</v>
       </c>
       <c r="N122" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="O122" s="2"/>
       <c r="P122" s="2"/>
@@ -5869,74 +5934,28 @@
         <v>44594</v>
       </c>
       <c r="E123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F123">
         <v>0</v>
       </c>
       <c r="G123">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H123">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="I123">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J123">
-        <v>9</v>
-      </c>
-      <c r="K123">
-        <v>8</v>
-      </c>
-      <c r="L123">
-        <v>8</v>
-      </c>
-      <c r="M123">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="N123" t="s">
         <v>15</v>
       </c>
       <c r="O123" s="2"/>
       <c r="P123" s="2"/>
-    </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A124">
-        <v>62</v>
-      </c>
-      <c r="C124" s="1">
-        <v>44589</v>
-      </c>
-      <c r="D124" s="1">
-        <v>44594</v>
-      </c>
-      <c r="E124" t="s">
-        <v>122</v>
-      </c>
-      <c r="F124">
-        <v>0</v>
-      </c>
-      <c r="G124">
-        <v>6</v>
-      </c>
-      <c r="H124">
-        <v>33</v>
-      </c>
-      <c r="I124">
-        <v>10</v>
-      </c>
-      <c r="J124">
-        <v>33</v>
-      </c>
-      <c r="K124" t="s">
-        <v>120</v>
-      </c>
-      <c r="N124" t="s">
-        <v>15</v>
-      </c>
-      <c r="O124" s="2"/>
-      <c r="P124" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>